<commit_message>
Client now communicates with GUI
</commit_message>
<xml_diff>
--- a/server/data/user_data.xlsx
+++ b/server/data/user_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/ljndan001_myuct_ac_za/Documents/1- Courses/CSC3002F/Assignments/ass1/database/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/ljndan001_myuct_ac_za/Documents/1- Courses/CSC3002F/Assignments/ass1/server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC104877F15E584A5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CB38254-C107-4306-8FCD-109A857CA1CD}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABDACC104877F15E584A5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D3EEA76-C62F-4527-AE46-A3216B41A17F}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,92 +35,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>user_id</t>
   </si>
   <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
     <t>LJNDAN001</t>
   </si>
   <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Le Jeune</t>
-  </si>
-  <si>
-    <t>Derick</t>
-  </si>
-  <si>
-    <t>Pena</t>
-  </si>
-  <si>
-    <t>Rayne</t>
-  </si>
-  <si>
-    <t>Meadows</t>
-  </si>
-  <si>
-    <t>Kelsie</t>
-  </si>
-  <si>
-    <t>Bonilla</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Lambert</t>
-  </si>
-  <si>
-    <t>Edith</t>
-  </si>
-  <si>
-    <t>Romero</t>
-  </si>
-  <si>
-    <t>Javion</t>
-  </si>
-  <si>
-    <t>Blanchard</t>
-  </si>
-  <si>
-    <t>Quintin</t>
-  </si>
-  <si>
-    <t>House</t>
-  </si>
-  <si>
-    <t>Alvaro</t>
-  </si>
-  <si>
-    <t>Tucker</t>
-  </si>
-  <si>
-    <t>Philip</t>
-  </si>
-  <si>
-    <t>Palmer</t>
-  </si>
-  <si>
-    <t>Aliana</t>
-  </si>
-  <si>
-    <t>Charles</t>
-  </si>
-  <si>
-    <t>Javon</t>
-  </si>
-  <si>
-    <t>Burns</t>
-  </si>
-  <si>
     <t>ip_address</t>
   </si>
   <si>
@@ -191,6 +113,12 @@
   </si>
   <si>
     <t>JAVBUR009</t>
+  </si>
+  <si>
+    <t>server_port</t>
+  </si>
+  <si>
+    <t>online_status</t>
   </si>
 </sst>
 </file>
@@ -511,7 +439,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,181 +449,181 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
+      <c r="C2">
+        <v>1200</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1200</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1200</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1200</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1200</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>1200</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>1200</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1200</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>1200</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>1200</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>1200</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>